<commit_message>
fixed data entry errors
</commit_message>
<xml_diff>
--- a/raw_data/KEEN ONE/Byrnes/2014/Calf Data Entry 2014/Calf Site Info 2014.xlsx
+++ b/raw_data/KEEN ONE/Byrnes/2014/Calf Data Entry 2014/Calf Site Info 2014.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="56">
   <si>
     <t>Transect 2</t>
   </si>
@@ -184,6 +184,15 @@
   <si>
     <t>visibility marked 1-2</t>
   </si>
+  <si>
+    <t>Calf Island</t>
+  </si>
+  <si>
+    <t>Boston Harbor Island</t>
+  </si>
+  <si>
+    <t>Byrnes</t>
+  </si>
 </sst>
 </file>
 
@@ -234,8 +243,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="63">
+  <cellStyleXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -316,7 +331,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="63">
+  <cellStyles count="69">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -348,6 +363,9 @@
     <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -379,6 +397,9 @@
     <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -779,7 +800,7 @@
   <dimension ref="A1:Q18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L21" sqref="L21"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -851,7 +872,15 @@
       </c>
     </row>
     <row r="2" spans="1:17">
-      <c r="B2"/>
+      <c r="A2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" t="s">
+        <v>53</v>
+      </c>
       <c r="D2" s="4" t="s">
         <v>3</v>
       </c>
@@ -871,13 +900,13 @@
         <v>42.346339999999998</v>
       </c>
       <c r="J2">
-        <v>70.892499999999998</v>
+        <v>-70.892499999999998</v>
       </c>
       <c r="K2">
         <v>42.345970000000001</v>
       </c>
       <c r="L2">
-        <v>70.892510000000001</v>
+        <v>-70.892510000000001</v>
       </c>
       <c r="M2">
         <v>7.4</v>
@@ -893,7 +922,15 @@
       </c>
     </row>
     <row r="3" spans="1:17">
-      <c r="B3"/>
+      <c r="A3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" t="s">
+        <v>53</v>
+      </c>
       <c r="D3" s="4" t="s">
         <v>0</v>
       </c>
@@ -913,13 +950,13 @@
         <v>42.344160000000002</v>
       </c>
       <c r="J3">
-        <v>70.89385</v>
+        <v>-70.89385</v>
       </c>
       <c r="K3">
         <v>42.344050000000003</v>
       </c>
       <c r="L3">
-        <v>70.894319999999993</v>
+        <v>-70.894319999999993</v>
       </c>
       <c r="M3">
         <v>7.6</v>
@@ -935,7 +972,15 @@
       </c>
     </row>
     <row r="4" spans="1:17">
-      <c r="B4"/>
+      <c r="A4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" t="s">
+        <v>53</v>
+      </c>
       <c r="D4" s="4" t="s">
         <v>1</v>
       </c>
@@ -955,13 +1000,13 @@
         <v>42.342950000000002</v>
       </c>
       <c r="J4">
-        <v>70.893270000000001</v>
+        <v>-70.893270000000001</v>
       </c>
       <c r="K4" s="3">
         <v>42.342959999999998</v>
       </c>
       <c r="L4">
-        <v>70.893749999999997</v>
+        <v>-70.893749999999997</v>
       </c>
       <c r="M4">
         <v>8.5</v>
@@ -980,8 +1025,15 @@
       </c>
     </row>
     <row r="5" spans="1:17" s="1" customFormat="1">
-      <c r="B5"/>
-      <c r="C5"/>
+      <c r="A5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5" t="s">
+        <v>53</v>
+      </c>
       <c r="D5" s="4" t="s">
         <v>2</v>
       </c>
@@ -1001,13 +1053,13 @@
         <v>42.340530000000001</v>
       </c>
       <c r="J5">
-        <v>70.893619999999999</v>
+        <v>-70.893619999999999</v>
       </c>
       <c r="K5" s="3">
         <v>42.340850000000003</v>
       </c>
       <c r="L5" s="3">
-        <v>70.893749999999997</v>
+        <v>-70.893749999999997</v>
       </c>
       <c r="M5" s="3">
         <v>8.1</v>

</xml_diff>